<commit_message>
save usertime in dbs
将原来form的形式改写成了ajax，在获取答案时jquery失败，最后用了原生的js代码，question页面所有数据均通过ajax发送，result通过get得到结果，但get只是一个展现数据通过参数userid和goal获得，
</commit_message>
<xml_diff>
--- a/question.xlsx
+++ b/question.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17301"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="333">
   <si>
     <t>马列主义、毛泽东思想</t>
   </si>
@@ -1843,6 +1843,110 @@
   </si>
   <si>
     <t>三个月</t>
+  </si>
+  <si>
+    <t>全面推进惩治和预防腐败体系建设，做到干部清正、政府清廉、()，反映了党推进反腐倡廉建设的坚定决心，对于提高党的建设科学化水平，凝聚党心民心，具有重要的指导意义。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>新时期党的干部工作的重要指导方针是( )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党章规定的各项纪律都必须严格遵守和执行，而最首要、最核心的就是要严格遵守和执行党的( )</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>( )是马克思主义政党的基本政治观点和根本工作路线。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国共产党是中国工人阶级的先锋队，同时是( )，是中国特色社会主义事业的领导核心，代表中国先进生产力的发展要求，代表中国先进文化的前进方向，代表中国最广大人民的根本利益。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党的最高理想和最终目标是( )。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党的根本宗旨是( )。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>马克思列宁主义揭示了( )，它的基本原理是正确的，具有强大的生命力。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>我国正处于并将长期处于( )。这是在经济文化落后的中国建设社会主义现代化不可逾越的历史阶段，需要上百年的时间。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国共产党在社会主义初级阶段的( )是：领导和团结全国各族人民，以经济建设为中心，坚持四项基本原则，坚持改革开放，自力更生，艰苦创业，为把我国建设成为富强、民主、文明的社会主义现代化国家而奋斗。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党的最高领导机关，是( )和它所产生的中央委员会。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党的领导主要是( )的领导。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党的思想路线是一切从实际出发，理论联系实际，( )，在实践中检验真理和发展真理。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>民主集中制是民主基础上的集中和集中指导下的民主相结合。它既是党的( )，也是群众路线在党的生活中的运用。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>我们党的最大政治优势是( )，党执政后的最大危险是脱离群众。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在现阶段，我国社会的( )是人民日益增长的物质文化需要同落后的社会生产之间的矛盾。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>必须尊重劳动、尊重知识、尊重人才、( )，做到发展为了人民、发展依靠人民、发展成果由人民共享。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党员必须自觉遵守党的纪律，模范遵守( )，严格保守党和国家的秘密，执行党的决定，服从组织分配，积极完成党的任务。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>预备党员的( )同正式党员一样。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>党员如果没有正当理由，连续( )不参加党的组织生活，或不交纳党费，或不做党所分配的工作，就被认为是自行脱党。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2219,10 +2323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2233,1140 +2337,1220 @@
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>106</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>307</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B56" s="1" t="s">
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="B58" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B59" s="1" t="s">
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>212</v>
       </c>
     </row>

</xml_diff>